<commit_message>
Paper Validado - EndersGranger
</commit_message>
<xml_diff>
--- a/Proyecto Interno/working-papers/working-paper-1225/m1/output/121225_m1_metrics.xlsx
+++ b/Proyecto Interno/working-papers/working-paper-1225/m1/output/121225_m1_metrics.xlsx
@@ -419,13 +419,13 @@
         <v>511.9024968713391</v>
       </c>
       <c r="F2">
-        <v>0.1519841097208292</v>
+        <v>15.19841097208292</v>
       </c>
       <c r="G2">
-        <v>0.1128067981092468</v>
+        <v>11.28067981092468</v>
       </c>
       <c r="H2">
-        <v>0.2019220774568518</v>
+        <v>20.19220774568518</v>
       </c>
     </row>
     <row r="3">
@@ -447,13 +447,13 @@
         <v>188.0703068058746</v>
       </c>
       <c r="F3">
-        <v>0.221848056097041</v>
+        <v>22.1848056097041</v>
       </c>
       <c r="G3">
-        <v>0.1585500179346827</v>
+        <v>15.85500179346827</v>
       </c>
       <c r="H3">
-        <v>0.1817229735814395</v>
+        <v>18.17229735814395</v>
       </c>
     </row>
     <row r="4">
@@ -475,13 +475,13 @@
         <v>408.2447965918637</v>
       </c>
       <c r="F4">
-        <v>0.2518034097536233</v>
+        <v>25.18034097536233</v>
       </c>
       <c r="G4">
-        <v>0.1741506851534091</v>
+        <v>17.41506851534091</v>
       </c>
       <c r="H4">
-        <v>0.2122155844301545</v>
+        <v>21.22155844301545</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +503,13 @@
         <v>75.11440245195026</v>
       </c>
       <c r="F5">
-        <v>0.0527916477348675</v>
+        <v>5.27916477348675</v>
       </c>
       <c r="G5">
-        <v>0.04506897087883811</v>
+        <v>4.506897087883812</v>
       </c>
       <c r="H5">
-        <v>0.04561136373877261</v>
+        <v>4.561136373877261</v>
       </c>
     </row>
     <row r="6">
@@ -531,13 +531,13 @@
         <v>2390.750225207094</v>
       </c>
       <c r="F6">
-        <v>0.2694410142514</v>
+        <v>26.94410142514</v>
       </c>
       <c r="G6">
-        <v>0.2545746006067922</v>
+        <v>25.45746006067922</v>
       </c>
       <c r="H6">
-        <v>0.3856949291003141</v>
+        <v>38.56949291003141</v>
       </c>
     </row>
     <row r="7">
@@ -559,13 +559,13 @@
         <v>50.5558884351132</v>
       </c>
       <c r="F7">
-        <v>0.07149115238474917</v>
+        <v>7.149115238474916</v>
       </c>
       <c r="G7">
-        <v>0.02291147405969096</v>
+        <v>2.291147405969096</v>
       </c>
       <c r="H7">
-        <v>0.03614557692292512</v>
+        <v>3.614557692292512</v>
       </c>
     </row>
     <row r="8">
@@ -587,13 +587,13 @@
         <v>141.2307426671682</v>
       </c>
       <c r="F8">
-        <v>0.02315121723786156</v>
+        <v>2.315121723786156</v>
       </c>
       <c r="G8">
-        <v>0.01921182557489114</v>
+        <v>1.921182557489114</v>
       </c>
       <c r="H8">
-        <v>0.0196336881630132</v>
+        <v>1.96336881630132</v>
       </c>
     </row>
     <row r="9">
@@ -615,13 +615,13 @@
         <v>263.8642567134933</v>
       </c>
       <c r="F9">
-        <v>0.06002705593346363</v>
+        <v>6.002705593346363</v>
       </c>
       <c r="G9">
-        <v>0.04872461079497119</v>
+        <v>4.872461079497119</v>
       </c>
       <c r="H9">
-        <v>0.03494767628969545</v>
+        <v>3.494767628969545</v>
       </c>
     </row>
     <row r="10">
@@ -643,13 +643,13 @@
         <v>46.01479267837701</v>
       </c>
       <c r="F10">
-        <v>0.09978274906507757</v>
+        <v>9.978274906507757</v>
       </c>
       <c r="G10">
-        <v>0.03485621142179225</v>
+        <v>3.485621142179224</v>
       </c>
       <c r="H10">
-        <v>0.02637161378466043</v>
+        <v>2.637161378466043</v>
       </c>
     </row>
     <row r="11">
@@ -671,13 +671,13 @@
         <v>115.5451743340055</v>
       </c>
       <c r="F11">
-        <v>0.2223878870576208</v>
+        <v>22.23878870576208</v>
       </c>
       <c r="G11">
-        <v>0.1300307168782545</v>
+        <v>13.00307168782545</v>
       </c>
       <c r="H11">
-        <v>0.06291312763471328</v>
+        <v>6.291312763471328</v>
       </c>
     </row>
     <row r="12">
@@ -699,13 +699,13 @@
         <v>113.5801501354039</v>
       </c>
       <c r="F12">
-        <v>0.1338541273106831</v>
+        <v>13.38541273106831</v>
       </c>
       <c r="G12">
-        <v>0.1050207652725773</v>
+        <v>10.50207652725773</v>
       </c>
       <c r="H12">
-        <v>0.1010928992396388</v>
+        <v>10.10928992396388</v>
       </c>
     </row>
     <row r="13">
@@ -727,13 +727,13 @@
         <v>358.4733379753175</v>
       </c>
       <c r="F13">
-        <v>0.1631598097150618</v>
+        <v>16.31598097150618</v>
       </c>
       <c r="G13">
-        <v>0.09882517727544861</v>
+        <v>9.882517727544862</v>
       </c>
       <c r="H13">
-        <v>0.04071642118704667</v>
+        <v>4.071642118704666</v>
       </c>
     </row>
     <row r="14">
@@ -755,13 +755,13 @@
         <v>98.97315345448406</v>
       </c>
       <c r="F14">
-        <v>0.04163567609648925</v>
+        <v>4.163567609648925</v>
       </c>
       <c r="G14">
-        <v>0.02114766979905234</v>
+        <v>2.114766979905234</v>
       </c>
       <c r="H14">
-        <v>0.01072579099136556</v>
+        <v>1.072579099136556</v>
       </c>
     </row>
     <row r="15">
@@ -783,13 +783,13 @@
         <v>548.3731200461323</v>
       </c>
       <c r="F15">
-        <v>0.0504791988329356</v>
+        <v>5.047919883293559</v>
       </c>
       <c r="G15">
-        <v>0.03049751897340255</v>
+        <v>3.049751897340255</v>
       </c>
       <c r="H15">
-        <v>0.08159585106099232</v>
+        <v>8.159585106099232</v>
       </c>
     </row>
     <row r="16">
@@ -811,13 +811,13 @@
         <v>730.3457343338259</v>
       </c>
       <c r="F16">
-        <v>0.04752081153783693</v>
+        <v>4.752081153783693</v>
       </c>
       <c r="G16">
-        <v>0.05863028590592249</v>
+        <v>5.86302859059225</v>
       </c>
       <c r="H16">
-        <v>0.1081322322707899</v>
+        <v>10.81322322707899</v>
       </c>
     </row>
     <row r="17">
@@ -839,13 +839,13 @@
         <v>535.8792304740862</v>
       </c>
       <c r="F17">
-        <v>0.02906188102721021</v>
+        <v>2.906188102721021</v>
       </c>
       <c r="G17">
-        <v>0.02609742145623272</v>
+        <v>2.609742145623272</v>
       </c>
       <c r="H17">
-        <v>0.05923386592302139</v>
+        <v>5.923386592302139</v>
       </c>
     </row>
     <row r="18">
@@ -867,13 +867,13 @@
         <v>83.76949995307037</v>
       </c>
       <c r="F18">
-        <v>0.1286435674529897</v>
+        <v>12.86435674529897</v>
       </c>
       <c r="G18">
-        <v>0.0198568925521506</v>
+        <v>1.98568925521506</v>
       </c>
       <c r="H18">
-        <v>0.02208199961591997</v>
+        <v>2.208199961591997</v>
       </c>
     </row>
     <row r="19">
@@ -895,13 +895,13 @@
         <v>418.2833208372813</v>
       </c>
       <c r="F19">
-        <v>0.07561418302633849</v>
+        <v>7.561418302633848</v>
       </c>
       <c r="G19">
-        <v>0.03684235604288356</v>
+        <v>3.684235604288356</v>
       </c>
       <c r="H19">
-        <v>0.03690304546691736</v>
+        <v>3.690304546691736</v>
       </c>
     </row>
     <row r="20">
@@ -923,13 +923,13 @@
         <v>883.8145325047943</v>
       </c>
       <c r="F20">
-        <v>0.03372239880283976</v>
+        <v>3.372239880283976</v>
       </c>
       <c r="G20">
-        <v>0.02603357193310758</v>
+        <v>2.603357193310758</v>
       </c>
       <c r="H20">
-        <v>0.1179357610474785</v>
+        <v>11.79357610474785</v>
       </c>
     </row>
     <row r="21">
@@ -951,13 +951,13 @@
         <v>1156.665396421299</v>
       </c>
       <c r="F21">
-        <v>0.0937662173736403</v>
+        <v>9.376621737364029</v>
       </c>
       <c r="G21">
-        <v>0.1004174695246989</v>
+        <v>10.04174695246989</v>
       </c>
       <c r="H21">
-        <v>0.1181307784216945</v>
+        <v>11.81307784216945</v>
       </c>
     </row>
     <row r="22">
@@ -979,13 +979,13 @@
         <v>1801.549147063886</v>
       </c>
       <c r="F22">
-        <v>0.02161637299665416</v>
+        <v>2.161637299665416</v>
       </c>
       <c r="G22">
-        <v>0.09474497320227114</v>
+        <v>9.474497320227114</v>
       </c>
       <c r="H22">
-        <v>0.2032731633059486</v>
+        <v>20.32731633059486</v>
       </c>
     </row>
     <row r="23">
@@ -1007,13 +1007,13 @@
         <v>1265.692647927591</v>
       </c>
       <c r="F23">
-        <v>0.01649863711727622</v>
+        <v>1.649863711727622</v>
       </c>
       <c r="G23">
-        <v>0.1004321600661222</v>
+        <v>10.04321600661222</v>
       </c>
       <c r="H23">
-        <v>0.142523668528585</v>
+        <v>14.2523668528585</v>
       </c>
     </row>
     <row r="24">
@@ -1035,13 +1035,13 @@
         <v>349.3405010594499</v>
       </c>
       <c r="F24">
-        <v>0.2193139473861287</v>
+        <v>21.93139473861287</v>
       </c>
       <c r="G24">
-        <v>0.1751957353340109</v>
+        <v>17.51957353340109</v>
       </c>
       <c r="H24">
-        <v>0.2268860462904709</v>
+        <v>22.68860462904709</v>
       </c>
     </row>
     <row r="25">
@@ -1063,13 +1063,13 @@
         <v>466.1344954407484</v>
       </c>
       <c r="F25">
-        <v>0.07587379346351478</v>
+        <v>7.587379346351478</v>
       </c>
       <c r="G25">
-        <v>0.1071866732253406</v>
+        <v>10.71866732253406</v>
       </c>
       <c r="H25">
-        <v>0.4045175292630261</v>
+        <v>40.45175292630262</v>
       </c>
     </row>
     <row r="26">
@@ -1091,13 +1091,13 @@
         <v>407.6211992152776</v>
       </c>
       <c r="F26">
-        <v>0.2281016626243452</v>
+        <v>22.81016626243452</v>
       </c>
       <c r="G26">
-        <v>0.1672017094568232</v>
+        <v>16.72017094568232</v>
       </c>
       <c r="H26">
-        <v>0.2789083634438168</v>
+        <v>27.89083634438168</v>
       </c>
     </row>
     <row r="27">
@@ -1119,13 +1119,13 @@
         <v>276.2478735340161</v>
       </c>
       <c r="F27">
-        <v>0.3221808273160891</v>
+        <v>32.21808273160891</v>
       </c>
       <c r="G27">
-        <v>0.1748274164103151</v>
+        <v>17.48274164103151</v>
       </c>
       <c r="H27">
-        <v>0.1741533991571239</v>
+        <v>17.41533991571239</v>
       </c>
     </row>
     <row r="28">
@@ -1147,13 +1147,13 @@
         <v>247.5859838433221</v>
       </c>
       <c r="F28">
-        <v>0.1020635304471567</v>
+        <v>10.20635304471567</v>
       </c>
       <c r="G28">
-        <v>0.09770810521319853</v>
+        <v>9.770810521319854</v>
       </c>
       <c r="H28">
-        <v>0.1331259052710733</v>
+        <v>13.31259052710733</v>
       </c>
     </row>
     <row r="29">
@@ -1175,13 +1175,13 @@
         <v>683.5733972343269</v>
       </c>
       <c r="F29">
-        <v>0.1160679475049154</v>
+        <v>11.60679475049154</v>
       </c>
       <c r="G29">
-        <v>0.07070952147817569</v>
+        <v>7.070952147817569</v>
       </c>
       <c r="H29">
-        <v>0.1388246738551676</v>
+        <v>13.88246738551676</v>
       </c>
     </row>
     <row r="30">
@@ -1203,13 +1203,13 @@
         <v>277.1142403269077</v>
       </c>
       <c r="F30">
-        <v>0.1341909278716169</v>
+        <v>13.41909278716169</v>
       </c>
       <c r="G30">
-        <v>0.1140359766686179</v>
+        <v>11.40359766686179</v>
       </c>
       <c r="H30">
-        <v>0.1743242789750115</v>
+        <v>17.43242789750115</v>
       </c>
     </row>
     <row r="31">
@@ -1231,13 +1231,13 @@
         <v>29.12619253942442</v>
       </c>
       <c r="F31">
-        <v>0.01472035587145883</v>
+        <v>1.472035587145883</v>
       </c>
       <c r="G31">
-        <v>0.0104307200262051</v>
+        <v>1.04307200262051</v>
       </c>
       <c r="H31">
-        <v>0.01724332329499565</v>
+        <v>1.724332329499565</v>
       </c>
     </row>
     <row r="32">
@@ -1259,13 +1259,13 @@
         <v>268.4347505720562</v>
       </c>
       <c r="F32">
-        <v>0.1015701878819195</v>
+        <v>10.15701878819195</v>
       </c>
       <c r="G32">
-        <v>0.1209952131616968</v>
+        <v>12.09952131616968</v>
       </c>
       <c r="H32">
-        <v>0.1490944460943054</v>
+        <v>14.90944460943054</v>
       </c>
     </row>
     <row r="33">
@@ -1287,13 +1287,13 @@
         <v>266.0877557536531</v>
       </c>
       <c r="F33">
-        <v>0.01469844368652982</v>
+        <v>1.469844368652982</v>
       </c>
       <c r="G33">
-        <v>0.0441399271340812</v>
+        <v>4.41399271340812</v>
       </c>
       <c r="H33">
-        <v>0.08732750308096007</v>
+        <v>8.732750308096007</v>
       </c>
     </row>
     <row r="34">
@@ -1315,13 +1315,13 @@
         <v>185.5512279059814</v>
       </c>
       <c r="F34">
-        <v>0.02708448399930673</v>
+        <v>2.708448399930673</v>
       </c>
       <c r="G34">
-        <v>0.0169836073754897</v>
+        <v>1.69836073754897</v>
       </c>
       <c r="H34">
-        <v>0.05149724481289829</v>
+        <v>5.149724481289828</v>
       </c>
     </row>
     <row r="35">
@@ -1343,13 +1343,13 @@
         <v>142.4498942012124</v>
       </c>
       <c r="F35">
-        <v>0.01304238961434247</v>
+        <v>1.304238961434247</v>
       </c>
       <c r="G35">
-        <v>0.01337365720910927</v>
+        <v>1.337365720910927</v>
       </c>
       <c r="H35">
-        <v>0.04113727905290847</v>
+        <v>4.113727905290847</v>
       </c>
     </row>
     <row r="36">
@@ -1371,13 +1371,13 @@
         <v>64.11784074325801</v>
       </c>
       <c r="F36">
-        <v>0.01849777822694286</v>
+        <v>1.849777822694286</v>
       </c>
       <c r="G36">
-        <v>0.01420892164738398</v>
+        <v>1.420892164738398</v>
       </c>
       <c r="H36">
-        <v>0.01704149202291591</v>
+        <v>1.704149202291591</v>
       </c>
     </row>
     <row r="37">
@@ -1399,13 +1399,13 @@
         <v>212.4618958250316</v>
       </c>
       <c r="F37">
-        <v>0.02169912074950437</v>
+        <v>2.169912074950437</v>
       </c>
       <c r="G37">
-        <v>0.01858045365251591</v>
+        <v>1.858045365251591</v>
       </c>
       <c r="H37">
-        <v>0.01537937070537711</v>
+        <v>1.537937070537711</v>
       </c>
     </row>
     <row r="38">
@@ -1427,13 +1427,13 @@
         <v>149.414555529036</v>
       </c>
       <c r="F38">
-        <v>0.1336292953590754</v>
+        <v>13.36292953590754</v>
       </c>
       <c r="G38">
-        <v>0.09910255990775613</v>
+        <v>9.910255990775612</v>
       </c>
       <c r="H38">
-        <v>0.1389893081486988</v>
+        <v>13.89893081486988</v>
       </c>
     </row>
     <row r="39">
@@ -1455,13 +1455,13 @@
         <v>229.7805135980329</v>
       </c>
       <c r="F39">
-        <v>0.05894784454621929</v>
+        <v>5.894784454621929</v>
       </c>
       <c r="G39">
-        <v>0.0645613207453232</v>
+        <v>6.45613207453232</v>
       </c>
       <c r="H39">
-        <v>0.08614594509764721</v>
+        <v>8.614594509764721</v>
       </c>
     </row>
     <row r="40">
@@ -1483,13 +1483,13 @@
         <v>421.6259447259587</v>
       </c>
       <c r="F40">
-        <v>0.2210212105495471</v>
+        <v>22.10212105495471</v>
       </c>
       <c r="G40">
-        <v>0.2293450202218624</v>
+        <v>22.93450202218624</v>
       </c>
       <c r="H40">
-        <v>0.3347581576960805</v>
+        <v>33.47581576960805</v>
       </c>
     </row>
     <row r="41">
@@ -1511,13 +1511,13 @@
         <v>799.960099874245</v>
       </c>
       <c r="F41">
-        <v>0.1760704769500333</v>
+        <v>17.60704769500333</v>
       </c>
       <c r="G41">
-        <v>0.12823373032992</v>
+        <v>12.823373032992</v>
       </c>
       <c r="H41">
-        <v>0.05337420567126535</v>
+        <v>5.337420567126535</v>
       </c>
     </row>
     <row r="42">
@@ -1539,13 +1539,13 @@
         <v>213.873092900844</v>
       </c>
       <c r="F42">
-        <v>0.1336370497878213</v>
+        <v>13.36370497878213</v>
       </c>
       <c r="G42">
-        <v>0.09253462099325151</v>
+        <v>9.253462099325152</v>
       </c>
       <c r="H42">
-        <v>0.1172359953151103</v>
+        <v>11.72359953151103</v>
       </c>
     </row>
     <row r="43">
@@ -1567,13 +1567,13 @@
         <v>715.2440284482275</v>
       </c>
       <c r="F43">
-        <v>0.2764106529560207</v>
+        <v>27.64106529560207</v>
       </c>
       <c r="G43">
-        <v>0.2719601154176929</v>
+        <v>27.19601154176929</v>
       </c>
       <c r="H43">
-        <v>0.4038024505521325</v>
+        <v>40.38024505521325</v>
       </c>
     </row>
     <row r="44">
@@ -1595,13 +1595,13 @@
         <v>461.4149468835211</v>
       </c>
       <c r="F44">
-        <v>0.2867894253915908</v>
+        <v>28.67894253915908</v>
       </c>
       <c r="G44">
-        <v>0.1774349007865237</v>
+        <v>17.74349007865237</v>
       </c>
       <c r="H44">
-        <v>0.3187494455221067</v>
+        <v>31.87494455221067</v>
       </c>
     </row>
     <row r="45">
@@ -1623,13 +1623,13 @@
         <v>187.2303406569755</v>
       </c>
       <c r="F45">
-        <v>0.02599236250157075</v>
+        <v>2.599236250157075</v>
       </c>
       <c r="G45">
-        <v>0.0264752074428098</v>
+        <v>2.64752074428098</v>
       </c>
       <c r="H45">
-        <v>0.05133972114440864</v>
+        <v>5.133972114440864</v>
       </c>
     </row>
     <row r="46">
@@ -1651,13 +1651,13 @@
         <v>232.290575513825</v>
       </c>
       <c r="F46">
-        <v>0.05480249813750043</v>
+        <v>5.480249813750042</v>
       </c>
       <c r="G46">
-        <v>0.04727757299025933</v>
+        <v>4.727757299025933</v>
       </c>
       <c r="H46">
-        <v>0.05984723829771622</v>
+        <v>5.984723829771623</v>
       </c>
     </row>
     <row r="47">
@@ -1679,13 +1679,13 @@
         <v>878.5826799254633</v>
       </c>
       <c r="F47">
-        <v>0.102931396864232</v>
+        <v>10.2931396864232</v>
       </c>
       <c r="G47">
-        <v>0.1441974791260922</v>
+        <v>14.41974791260922</v>
       </c>
       <c r="H47">
-        <v>0.2340886426638768</v>
+        <v>23.40886426638768</v>
       </c>
     </row>
     <row r="48">
@@ -1707,13 +1707,13 @@
         <v>240.6626103040623</v>
       </c>
       <c r="F48">
-        <v>0.1882781450060252</v>
+        <v>18.82781450060252</v>
       </c>
       <c r="G48">
-        <v>0.1272707498057428</v>
+        <v>12.72707498057428</v>
       </c>
       <c r="H48">
-        <v>0.1099977452863461</v>
+        <v>10.99977452863461</v>
       </c>
     </row>
     <row r="49">
@@ -1735,13 +1735,13 @@
         <v>167.9166460945509</v>
       </c>
       <c r="F49">
-        <v>0.1798535845841979</v>
+        <v>17.98535845841979</v>
       </c>
       <c r="G49">
-        <v>0.08256863796427448</v>
+        <v>8.256863796427448</v>
       </c>
       <c r="H49">
-        <v>0.03986395891914929</v>
+        <v>3.986395891914929</v>
       </c>
     </row>
     <row r="50">
@@ -1763,13 +1763,13 @@
         <v>241.4235675547847</v>
       </c>
       <c r="F50">
-        <v>0.1719732542050645</v>
+        <v>17.19732542050645</v>
       </c>
       <c r="G50">
-        <v>0.1250958942780724</v>
+        <v>12.50958942780724</v>
       </c>
       <c r="H50">
-        <v>0.09175638102317807</v>
+        <v>9.175638102317807</v>
       </c>
     </row>
     <row r="51">
@@ -1791,13 +1791,13 @@
         <v>37.84220835976163</v>
       </c>
       <c r="F51">
-        <v>0.2327164071784693</v>
+        <v>23.27164071784692</v>
       </c>
       <c r="G51">
-        <v>0.05328580076068469</v>
+        <v>5.328580076068469</v>
       </c>
       <c r="H51">
-        <v>0.04205298765424881</v>
+        <v>4.205298765424882</v>
       </c>
     </row>
     <row r="52">
@@ -1819,13 +1819,13 @@
         <v>192.0368104821152</v>
       </c>
       <c r="F52">
-        <v>0.2704005270672092</v>
+        <v>27.04005270672092</v>
       </c>
       <c r="G52">
-        <v>0.215283028321591</v>
+        <v>21.52830283215911</v>
       </c>
       <c r="H52">
-        <v>0.1889551205022862</v>
+        <v>18.89551205022862</v>
       </c>
     </row>
     <row r="53">
@@ -1847,13 +1847,13 @@
         <v>134.6501479582044</v>
       </c>
       <c r="F53">
-        <v>0.2636190221532001</v>
+        <v>26.36190221532001</v>
       </c>
       <c r="G53">
-        <v>0.2184907206234001</v>
+        <v>21.84907206234001</v>
       </c>
       <c r="H53">
-        <v>0.1780455037083545</v>
+        <v>17.80455037083545</v>
       </c>
     </row>
     <row r="54">
@@ -1875,13 +1875,13 @@
         <v>242.2486703507989</v>
       </c>
       <c r="F54">
-        <v>0.05891285288121825</v>
+        <v>5.891285288121825</v>
       </c>
       <c r="G54">
-        <v>0.08533770240054457</v>
+        <v>8.533770240054457</v>
       </c>
       <c r="H54">
-        <v>0.1108339930799387</v>
+        <v>11.08339930799387</v>
       </c>
     </row>
     <row r="55">
@@ -1903,13 +1903,13 @@
         <v>348.7611563976278</v>
       </c>
       <c r="F55">
-        <v>0.1534938614322293</v>
+        <v>15.34938614322293</v>
       </c>
       <c r="G55">
-        <v>0.2454690146754461</v>
+        <v>24.54690146754461</v>
       </c>
       <c r="H55">
-        <v>0.4745081553873345</v>
+        <v>47.45081553873345</v>
       </c>
     </row>
     <row r="56">
@@ -1931,13 +1931,13 @@
         <v>189.1193790058087</v>
       </c>
       <c r="F56">
-        <v>0.05598949004801083</v>
+        <v>5.598949004801083</v>
       </c>
       <c r="G56">
-        <v>0.04947271441854392</v>
+        <v>4.947271441854392</v>
       </c>
       <c r="H56">
-        <v>0.2466147320632139</v>
+        <v>24.66147320632139</v>
       </c>
     </row>
     <row r="57">
@@ -1959,13 +1959,13 @@
         <v>211.2656131249121</v>
       </c>
       <c r="F57">
-        <v>0.1317211168637778</v>
+        <v>13.17211168637778</v>
       </c>
       <c r="G57">
-        <v>0.1845711355171027</v>
+        <v>18.45711355171027</v>
       </c>
       <c r="H57">
-        <v>0.3044631437555823</v>
+        <v>30.44631437555823</v>
       </c>
     </row>
     <row r="58">
@@ -1987,13 +1987,13 @@
         <v>448.3668450520643</v>
       </c>
       <c r="F58">
-        <v>0.1977955754652945</v>
+        <v>19.77955754652945</v>
       </c>
       <c r="G58">
-        <v>0.2005210410337412</v>
+        <v>20.05210410337412</v>
       </c>
       <c r="H58">
-        <v>0.3041924660237514</v>
+        <v>30.41924660237514</v>
       </c>
     </row>
     <row r="59">
@@ -2015,13 +2015,13 @@
         <v>433.6415964235396</v>
       </c>
       <c r="F59">
-        <v>0.2082305699703817</v>
+        <v>20.82305699703817</v>
       </c>
       <c r="G59">
-        <v>0.1997581055484863</v>
+        <v>19.97581055484863</v>
       </c>
       <c r="H59">
-        <v>0.2830010024306172</v>
+        <v>28.30010024306172</v>
       </c>
     </row>
     <row r="60">
@@ -2043,13 +2043,13 @@
         <v>241.709592459443</v>
       </c>
       <c r="F60">
-        <v>0.2251193027940099</v>
+        <v>22.51193027940099</v>
       </c>
       <c r="G60">
-        <v>0.2236391348196999</v>
+        <v>22.36391348196998</v>
       </c>
       <c r="H60">
-        <v>0.2694869587180028</v>
+        <v>26.94869587180028</v>
       </c>
     </row>
     <row r="61">
@@ -2071,13 +2071,13 @@
         <v>227.4679068309253</v>
       </c>
       <c r="F61">
-        <v>0.1678051411087724</v>
+        <v>16.78051411087724</v>
       </c>
       <c r="G61">
-        <v>0.2091440455110343</v>
+        <v>20.91440455110343</v>
       </c>
       <c r="H61">
-        <v>0.3018211420329024</v>
+        <v>30.18211420329024</v>
       </c>
     </row>
     <row r="62">
@@ -2099,13 +2099,13 @@
         <v>245.1340817267836</v>
       </c>
       <c r="F62">
-        <v>0.1656747253639325</v>
+        <v>16.56747253639325</v>
       </c>
       <c r="G62">
-        <v>0.2311005172079883</v>
+        <v>23.11005172079883</v>
       </c>
       <c r="H62">
-        <v>0.3251823604854958</v>
+        <v>32.51823604854957</v>
       </c>
     </row>
     <row r="63">
@@ -2127,13 +2127,13 @@
         <v>352.6791468570917</v>
       </c>
       <c r="F63">
-        <v>0.1992832573897891</v>
+        <v>19.92832573897891</v>
       </c>
       <c r="G63">
-        <v>0.3363237702633427</v>
+        <v>33.63237702633427</v>
       </c>
       <c r="H63">
-        <v>0.4593330608778467</v>
+        <v>45.93330608778467</v>
       </c>
     </row>
     <row r="64">
@@ -2155,13 +2155,13 @@
         <v>372.7422684403281</v>
       </c>
       <c r="F64">
-        <v>0.1911305470414221</v>
+        <v>19.11305470414221</v>
       </c>
       <c r="G64">
-        <v>0.1681786427766979</v>
+        <v>16.81786427766979</v>
       </c>
       <c r="H64">
-        <v>0.1171676760257564</v>
+        <v>11.71676760257564</v>
       </c>
     </row>
     <row r="65">
@@ -2183,13 +2183,13 @@
         <v>175.3868344571449</v>
       </c>
       <c r="F65">
-        <v>0.03355330289965456</v>
+        <v>3.355330289965456</v>
       </c>
       <c r="G65">
-        <v>0.02603873674412696</v>
+        <v>2.603873674412696</v>
       </c>
       <c r="H65">
-        <v>0.0305633975099419</v>
+        <v>3.05633975099419</v>
       </c>
     </row>
     <row r="66">
@@ -2211,13 +2211,13 @@
         <v>46.5640819490225</v>
       </c>
       <c r="F66">
-        <v>0.218591852706303</v>
+        <v>21.85918527063031</v>
       </c>
       <c r="G66">
-        <v>0.1339149222359535</v>
+        <v>13.39149222359535</v>
       </c>
       <c r="H66">
-        <v>0.05516476479199354</v>
+        <v>5.516476479199354</v>
       </c>
     </row>
     <row r="67">
@@ -2239,13 +2239,13 @@
         <v>69.16371261050027</v>
       </c>
       <c r="F67">
-        <v>0.05009128203785899</v>
+        <v>5.0091282037859</v>
       </c>
       <c r="G67">
-        <v>0.05292818962429675</v>
+        <v>5.292818962429675</v>
       </c>
       <c r="H67">
-        <v>0.08791674038277042</v>
+        <v>8.791674038277042</v>
       </c>
     </row>
     <row r="68">
@@ -2267,13 +2267,13 @@
         <v>169.007738510003</v>
       </c>
       <c r="F68">
-        <v>0.06429308537407454</v>
+        <v>6.429308537407453</v>
       </c>
       <c r="G68">
-        <v>0.04408812324060395</v>
+        <v>4.408812324060396</v>
       </c>
       <c r="H68">
-        <v>0.03542906984560831</v>
+        <v>3.542906984560831</v>
       </c>
     </row>
     <row r="69">
@@ -2295,13 +2295,13 @@
         <v>179.8119151166307</v>
       </c>
       <c r="F69">
-        <v>0.0252916469115123</v>
+        <v>2.52916469115123</v>
       </c>
       <c r="G69">
-        <v>0.01666428512856313</v>
+        <v>1.666428512856313</v>
       </c>
       <c r="H69">
-        <v>0.02110353417042136</v>
+        <v>2.110353417042136</v>
       </c>
     </row>
     <row r="70">
@@ -2323,13 +2323,13 @@
         <v>346.2316939836224</v>
       </c>
       <c r="F70">
-        <v>0.2136047287395646</v>
+        <v>21.36047287395646</v>
       </c>
       <c r="G70">
-        <v>0.2421059853592071</v>
+        <v>24.21059853592071</v>
       </c>
       <c r="H70">
-        <v>0.4207172656886821</v>
+        <v>42.07172656886821</v>
       </c>
     </row>
     <row r="71">
@@ -2351,13 +2351,13 @@
         <v>15.12126361709926</v>
       </c>
       <c r="F71">
-        <v>0.05178111733099722</v>
+        <v>5.178111733099722</v>
       </c>
       <c r="G71">
-        <v>0.02278834156542943</v>
+        <v>2.278834156542943</v>
       </c>
       <c r="H71">
-        <v>0.01987726919557737</v>
+        <v>1.987726919557737</v>
       </c>
     </row>
     <row r="72">
@@ -2379,13 +2379,13 @@
         <v>1228.403648746858</v>
       </c>
       <c r="F72">
-        <v>0.1094707162534506</v>
+        <v>10.94707162534506</v>
       </c>
       <c r="G72">
-        <v>0.0848197684163441</v>
+        <v>8.48197684163441</v>
       </c>
       <c r="H72">
-        <v>0.078579574575334</v>
+        <v>7.8579574575334</v>
       </c>
     </row>
     <row r="73">
@@ -2407,13 +2407,13 @@
         <v>383.2197152732053</v>
       </c>
       <c r="F73">
-        <v>0.1857198707624358</v>
+        <v>18.57198707624358</v>
       </c>
       <c r="G73">
-        <v>0.1909009562410861</v>
+        <v>19.09009562410861</v>
       </c>
       <c r="H73">
-        <v>0.2599084994602945</v>
+        <v>25.99084994602945</v>
       </c>
     </row>
     <row r="74">
@@ -2435,13 +2435,13 @@
         <v>237.4209946844574</v>
       </c>
       <c r="F74">
-        <v>0.1510466191720918</v>
+        <v>15.10466191720918</v>
       </c>
       <c r="G74">
-        <v>0.1417240072897671</v>
+        <v>14.17240072897671</v>
       </c>
       <c r="H74">
-        <v>0.2048008437415025</v>
+        <v>20.48008437415025</v>
       </c>
     </row>
     <row r="75">
@@ -2463,13 +2463,13 @@
         <v>469.0395952395173</v>
       </c>
       <c r="F75">
-        <v>0.408360434972011</v>
+        <v>40.8360434972011</v>
       </c>
       <c r="G75">
-        <v>0.3584347588964482</v>
+        <v>35.84347588964482</v>
       </c>
       <c r="H75">
-        <v>0.3787470303319111</v>
+        <v>37.87470303319112</v>
       </c>
     </row>
   </sheetData>
@@ -2512,7 +2512,7 @@
         <v>565.3923640032616</v>
       </c>
       <c r="C2">
-        <v>0.1290295865176274</v>
+        <v>12.90295865176275</v>
       </c>
     </row>
     <row r="3">
@@ -2525,7 +2525,7 @@
         <v>481.2113161894767</v>
       </c>
       <c r="C3">
-        <v>0.1123425292150635</v>
+        <v>11.23425292150636</v>
       </c>
     </row>
     <row r="4">
@@ -2538,7 +2538,7 @@
         <v>549.051144425219</v>
       </c>
       <c r="C4">
-        <v>0.1487198738081381</v>
+        <v>14.87198738081381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>